<commit_message>
Avoid infinite recursive RescanFieldNames on column insert (#1492)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Tables/ResizingTables.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Tables/ResizingTables.xlsx
@@ -9,6 +9,7 @@
     <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <x:sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <x:sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <x:si>
     <x:t>Index</x:t>
   </x:si>
@@ -97,6 +98,9 @@
   </x:si>
   <x:si>
     <x:t>73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Column4</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -193,6 +197,20 @@
     <x:tableColumn id="3" name="Character"/>
     <x:tableColumn id="4" name="String"/>
     <x:tableColumn id="5" name="Integer" totalsRowLabel="73"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table13" displayName="Table13" ref="B2:F13" totalsRowCount="1">
+  <x:autoFilter ref="B2:F12"/>
+  <x:tableColumns count="5">
+    <x:tableColumn id="1" name="Index" totalsRowLabel="Sum of Integer"/>
+    <x:tableColumn id="2" name="Character"/>
+    <x:tableColumn id="3" name="String"/>
+    <x:tableColumn id="4" name="Column4"/>
+    <x:tableColumn id="5" name="Integer" totalsRowFunction="sum"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -667,7 +685,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId7"/>
+    <x:tablePart r:id="rId8"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -684,7 +702,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.235425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="10.685425" style="0" customWidth="1"/>
@@ -865,7 +883,7 @@
     <x:firstFooter/>
   </x:headerFooter>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId8"/>
+    <x:tablePart r:id="rId9"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -882,7 +900,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="12.195425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.235425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="10.685425" style="0" customWidth="1"/>
@@ -1066,7 +1084,209 @@
     <x:firstFooter/>
   </x:headerFooter>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId9"/>
+    <x:tablePart r:id="rId10"/>
+  </x:tableParts>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F13"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="10.685425" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="2" spans="1:6">
+      <x:c r="B2" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="B3" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="B4" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="B5" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="B6" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="B7" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="B8" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="B9" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="n">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="B10" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="B11" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="n">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="B12" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="n">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="B13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F13" s="0">
+        <x:f>SUBTOTAL(109,[Integer])</x:f>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1">
+    <x:oddHeader/>
+    <x:oddFooter/>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
+  <x:tableParts count="1">
+    <x:tablePart r:id="rId11"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>